<commit_message>
Updated dataset with price column
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0211B1-9C70-46B9-A0D7-4E136D9F3A23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE393D2-A244-4C0D-9602-2EE29AECF6FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$16</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -507,6 +507,9 @@
   </si>
   <si>
     <t>TourdeFranceYellow</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -833,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,10 +851,11 @@
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="124.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -874,10 +878,13 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -899,11 +906,14 @@
       <c r="G2">
         <v>2020</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>1208.97</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -925,11 +935,14 @@
       <c r="G3">
         <v>2021</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>403.97</v>
+      </c>
+      <c r="I3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -951,11 +964,14 @@
       <c r="G4">
         <v>2020</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>1575.25</v>
+      </c>
+      <c r="I4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -977,11 +993,14 @@
       <c r="G5">
         <v>2020</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <v>1857.84</v>
+      </c>
+      <c r="I5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1003,11 +1022,14 @@
       <c r="G6">
         <v>2020</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6">
+        <v>1447.9</v>
+      </c>
+      <c r="I6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1029,11 +1051,14 @@
       <c r="G7">
         <v>2021</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7">
+        <v>1092.76</v>
+      </c>
+      <c r="I7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1055,11 +1080,14 @@
       <c r="G8">
         <v>2020</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <v>744.26</v>
+      </c>
+      <c r="I8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1081,11 +1109,14 @@
       <c r="G9">
         <v>2020</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9">
+        <v>1125.04</v>
+      </c>
+      <c r="I9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1107,11 +1138,14 @@
       <c r="G10">
         <v>2020</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10">
+        <v>607.82000000000005</v>
+      </c>
+      <c r="I10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1133,11 +1167,14 @@
       <c r="G11">
         <v>2020</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11">
+        <v>1762.82</v>
+      </c>
+      <c r="I11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1159,11 +1196,14 @@
       <c r="G13">
         <v>2021</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13">
+        <v>577.64</v>
+      </c>
+      <c r="I13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1185,11 +1225,14 @@
       <c r="G14">
         <v>2020</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14">
+        <v>1283.6300000000001</v>
+      </c>
+      <c r="I14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1211,11 +1254,14 @@
       <c r="G15">
         <v>2019</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15">
+        <v>1235.53</v>
+      </c>
+      <c r="I15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1237,11 +1283,14 @@
       <c r="G16">
         <v>2020</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16">
+        <v>1821.8</v>
+      </c>
+      <c r="I16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1263,11 +1312,14 @@
       <c r="G17">
         <v>2021</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17">
+        <v>1426.79</v>
+      </c>
+      <c r="I17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1289,11 +1341,14 @@
       <c r="G18">
         <v>2020</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18">
+        <v>379.34</v>
+      </c>
+      <c r="I18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1315,11 +1370,14 @@
       <c r="G19">
         <v>2019</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19">
+        <v>521.70000000000005</v>
+      </c>
+      <c r="I19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1341,11 +1399,14 @@
       <c r="G20">
         <v>2020</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20">
+        <v>1229.22</v>
+      </c>
+      <c r="I20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1367,11 +1428,14 @@
       <c r="G21">
         <v>2020</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21">
+        <v>676.88</v>
+      </c>
+      <c r="I21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -1393,11 +1457,14 @@
       <c r="G22">
         <v>2020</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22">
+        <v>364.45</v>
+      </c>
+      <c r="I22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1419,11 +1486,14 @@
       <c r="G24">
         <v>2020</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24">
+        <v>1429.11</v>
+      </c>
+      <c r="I24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1445,11 +1515,14 @@
       <c r="G25">
         <v>2020</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25">
+        <v>1092.3499999999999</v>
+      </c>
+      <c r="I25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1471,11 +1544,14 @@
       <c r="G26">
         <v>2020</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26">
+        <v>528.92999999999995</v>
+      </c>
+      <c r="I26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1497,11 +1573,14 @@
       <c r="G27">
         <v>2020</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27">
+        <v>1090.44</v>
+      </c>
+      <c r="I27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -1523,11 +1602,14 @@
       <c r="G28">
         <v>2020</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28">
+        <v>1849.42</v>
+      </c>
+      <c r="I28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1549,11 +1631,14 @@
       <c r="G29">
         <v>2020</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29">
+        <v>753.61</v>
+      </c>
+      <c r="I29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -1575,11 +1660,14 @@
       <c r="G30">
         <v>2020</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30">
+        <v>1573.85</v>
+      </c>
+      <c r="I30" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -1601,11 +1689,14 @@
       <c r="G31">
         <v>2021</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31">
+        <v>1801.22</v>
+      </c>
+      <c r="I31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -1627,11 +1718,14 @@
       <c r="G32">
         <v>2020</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32">
+        <v>587.66</v>
+      </c>
+      <c r="I32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -1653,11 +1747,14 @@
       <c r="G33">
         <v>2020</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33">
+        <v>1684.73</v>
+      </c>
+      <c r="I33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -1679,11 +1776,14 @@
       <c r="G35">
         <v>2021</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35">
+        <v>427.76</v>
+      </c>
+      <c r="I35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -1705,11 +1805,14 @@
       <c r="G36">
         <v>2021</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36">
+        <v>1359.8</v>
+      </c>
+      <c r="I36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -1731,11 +1834,14 @@
       <c r="G37">
         <v>2021</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37">
+        <v>819.61</v>
+      </c>
+      <c r="I37" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -1757,11 +1863,14 @@
       <c r="G38">
         <v>2020</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38">
+        <v>819.95</v>
+      </c>
+      <c r="I38" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -1783,11 +1892,14 @@
       <c r="G39">
         <v>2019</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39">
+        <v>452.75</v>
+      </c>
+      <c r="I39" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -1809,11 +1921,14 @@
       <c r="G40">
         <v>2021</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40">
+        <v>1107.67</v>
+      </c>
+      <c r="I40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>104</v>
       </c>
@@ -1835,11 +1950,14 @@
       <c r="G41">
         <v>2020</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41">
+        <v>1205.98</v>
+      </c>
+      <c r="I41" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -1861,11 +1979,14 @@
       <c r="G42">
         <v>2021</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42">
+        <v>1166.06</v>
+      </c>
+      <c r="I42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>113</v>
       </c>
@@ -1887,11 +2008,14 @@
       <c r="G43">
         <v>2022</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43">
+        <v>1653.37</v>
+      </c>
+      <c r="I43" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>115</v>
       </c>
@@ -1913,7 +2037,10 @@
       <c r="G44">
         <v>2020</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44">
+        <v>1581.64</v>
+      </c>
+      <c r="I44" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1926,10 +2053,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBAF722-6FF6-47E8-8911-72262127743F}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,82 +2064,292 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <f ca="1">RAND()*(2000-350)+350</f>
+        <v>877.87957536356907</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <f t="shared" ref="B2:B43" ca="1" si="0">RAND()*(2000-350)+350</f>
+        <v>581.24034097780225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1298.6371717057796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>463.95303202113587</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1735.070616811782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1208.0420997450346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1410.7275701972039</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>648.14718674247342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>578.00452573488678</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1245.6190099221055</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1435.6687308547127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1869.814297623928</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1675.298908191161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1303.4462312852572</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>363.96063657761772</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1490.0695134279913</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>1768.0163517392532</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>1590.1270518767369</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>1220.8920743991953</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>1349.1893892652342</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f t="shared" ca="1" si="0"/>
+        <v>1597.6158381411733</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" ca="1" si="0"/>
+        <v>786.03558231101931</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1046.8582600728764</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f t="shared" ca="1" si="0"/>
+        <v>959.06517249342835</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1277.4598680791332</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" ca="1" si="0"/>
+        <v>919.98545775370917</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f t="shared" ca="1" si="0"/>
+        <v>896.12976870053058</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f t="shared" ca="1" si="0"/>
+        <v>571.0723892973017</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" ca="1" si="0"/>
+        <v>1956.5233871824266</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f t="shared" ca="1" si="0"/>
+        <v>421.3541445933742</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f t="shared" ca="1" si="0"/>
+        <v>802.39479104973088</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" ca="1" si="0"/>
+        <v>1446.4748182649814</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" ca="1" si="0"/>
+        <v>518.48992646314218</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1322.8366291957575</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" ca="1" si="0"/>
+        <v>977.96062631390475</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" ca="1" si="0"/>
+        <v>1363.2000736165196</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" ca="1" si="0"/>
+        <v>717.39221279829314</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" ca="1" si="0"/>
+        <v>1966.5854545886291</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f t="shared" ca="1" si="0"/>
+        <v>1137.1256263448074</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f t="shared" ca="1" si="0"/>
+        <v>988.6636431659407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted colour field and included quantity values
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE393D2-A244-4C0D-9602-2EE29AECF6FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2722381E-7758-42F8-8B6F-5EB25487D157}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Quantity" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Quantity!$A$2:$A$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Haibike SDuro Hardseven 6.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Haibike </t>
-  </si>
-  <si>
     <t>https://tredz.azureedge.net/prodimg/226629-739869_1_Supersize.jpg</t>
   </si>
   <si>
@@ -452,64 +449,70 @@
     <t>Haibike</t>
   </si>
   <si>
-    <t>CarbonGrey</t>
-  </si>
-  <si>
-    <t>ChameleonTerra</t>
-  </si>
-  <si>
-    <t>TitaniumBlack</t>
-  </si>
-  <si>
-    <t>MetallicRed</t>
-  </si>
-  <si>
-    <t>GlossyBlue</t>
-  </si>
-  <si>
-    <t>MetallicBlack/TrekkingGreen</t>
-  </si>
-  <si>
-    <t>GlossCarbon/BlackChrome</t>
-  </si>
-  <si>
     <t>Green/Black</t>
   </si>
   <si>
-    <t>BlackPhantom/Yellow</t>
-  </si>
-  <si>
-    <t>MattGrey/Lime/Blue</t>
-  </si>
-  <si>
     <t>Black/Red/Black</t>
   </si>
   <si>
-    <t>SatinCarbon/Mint</t>
-  </si>
-  <si>
-    <t>Carbon/White/BoxRed</t>
-  </si>
-  <si>
     <t>Abalone/Black/Black</t>
   </si>
   <si>
-    <t>SparklingRed/Black</t>
-  </si>
-  <si>
-    <t>GlossYellow/GlossDeepBlue</t>
-  </si>
-  <si>
-    <t>NeonGreen</t>
-  </si>
-  <si>
-    <t>LightBlue/Red</t>
-  </si>
-  <si>
-    <t>TourdeFranceYellow</t>
-  </si>
-  <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Carbon_Grey</t>
+  </si>
+  <si>
+    <t>Chameleon_Terra</t>
+  </si>
+  <si>
+    <t>Titanium_Black</t>
+  </si>
+  <si>
+    <t>Metallic_Red</t>
+  </si>
+  <si>
+    <t>Glossy_Blue</t>
+  </si>
+  <si>
+    <t>Metallic_Black/Trekking_Green</t>
+  </si>
+  <si>
+    <t>Gloss_Carbon/Black_Chrome</t>
+  </si>
+  <si>
+    <t>Black_Phantom/Yellow</t>
+  </si>
+  <si>
+    <t>Matt_Grey/Lime/Blue</t>
+  </si>
+  <si>
+    <t>Satin_Carbon/Mint</t>
+  </si>
+  <si>
+    <t>Carbon/White/Box_Red</t>
+  </si>
+  <si>
+    <t>Sparkling_Red/Black</t>
+  </si>
+  <si>
+    <t>Gloss_Yellow/Gloss_Deep_Blue</t>
+  </si>
+  <si>
+    <t>Neon_Green</t>
+  </si>
+  <si>
+    <t>Light_Blue/Red</t>
+  </si>
+  <si>
+    <t>Tour_de_France_Yellow</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
@@ -553,9 +556,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,22 +870,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -895,10 +899,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -956,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -982,10 +986,10 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -1011,10 +1015,10 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -1043,7 +1047,7 @@
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -1072,7 +1076,7 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -1101,7 +1105,7 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -1127,7 +1131,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E10" t="s">
         <v>35</v>
@@ -1156,10 +1160,10 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -1185,10 +1189,10 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -1214,7 +1218,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E14" t="s">
         <v>43</v>
@@ -1243,10 +1247,10 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
@@ -1272,10 +1276,10 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -1304,7 +1308,7 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
@@ -1330,10 +1334,10 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -1359,10 +1363,10 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
@@ -1388,10 +1392,10 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -1417,7 +1421,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E21" t="s">
         <v>63</v>
@@ -1446,10 +1450,10 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
@@ -1475,7 +1479,7 @@
         <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
         <v>35</v>
@@ -1498,7 +1502,7 @@
         <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" t="s">
         <v>67</v>
@@ -1507,7 +1511,7 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F25" t="s">
         <v>9</v>
@@ -1519,12 +1523,12 @@
         <v>1092.3499999999999</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>52</v>
@@ -1533,10 +1537,10 @@
         <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
@@ -1548,12 +1552,12 @@
         <v>528.92999999999995</v>
       </c>
       <c r="I26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
         <v>42</v>
@@ -1562,10 +1566,10 @@
         <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27" t="s">
         <v>9</v>
@@ -1577,12 +1581,12 @@
         <v>1090.44</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -1591,10 +1595,10 @@
         <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F28" t="s">
         <v>9</v>
@@ -1606,12 +1610,12 @@
         <v>1849.42</v>
       </c>
       <c r="I28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
         <v>21</v>
@@ -1623,7 +1627,7 @@
         <v>156</v>
       </c>
       <c r="E29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
@@ -1635,12 +1639,12 @@
         <v>753.61</v>
       </c>
       <c r="I29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
         <v>62</v>
@@ -1649,10 +1653,10 @@
         <v>67</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
         <v>9</v>
@@ -1664,12 +1668,12 @@
         <v>1573.85</v>
       </c>
       <c r="I30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
         <v>48</v>
@@ -1681,7 +1685,7 @@
         <v>157</v>
       </c>
       <c r="E31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F31" t="s">
         <v>9</v>
@@ -1693,12 +1697,12 @@
         <v>1801.22</v>
       </c>
       <c r="I31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -1707,7 +1711,7 @@
         <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
         <v>43</v>
@@ -1722,12 +1726,12 @@
         <v>587.66</v>
       </c>
       <c r="I32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
         <v>69</v>
@@ -1736,10 +1740,10 @@
         <v>67</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
@@ -1751,24 +1755,24 @@
         <v>1684.73</v>
       </c>
       <c r="I33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F35" t="s">
         <v>9</v>
@@ -1780,24 +1784,24 @@
         <v>427.76</v>
       </c>
       <c r="I35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
         <v>96</v>
       </c>
-      <c r="B36" t="s">
-        <v>97</v>
-      </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F36" t="s">
         <v>9</v>
@@ -1809,24 +1813,24 @@
         <v>1359.8</v>
       </c>
       <c r="I36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D37" t="s">
         <v>158</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F37" t="s">
         <v>9</v>
@@ -1838,24 +1842,24 @@
         <v>819.61</v>
       </c>
       <c r="I37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B38" t="s">
         <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
         <v>159</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F38" t="s">
         <v>9</v>
@@ -1867,24 +1871,24 @@
         <v>819.95</v>
       </c>
       <c r="I38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
         <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F39" t="s">
         <v>9</v>
@@ -1896,24 +1900,24 @@
         <v>452.75</v>
       </c>
       <c r="I39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
         <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
@@ -1925,24 +1929,24 @@
         <v>1107.67</v>
       </c>
       <c r="I40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F41" t="s">
         <v>9</v>
@@ -1954,24 +1958,24 @@
         <v>1205.98</v>
       </c>
       <c r="I41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
       </c>
       <c r="E42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F42" t="s">
         <v>9</v>
@@ -1983,24 +1987,24 @@
         <v>1166.06</v>
       </c>
       <c r="I42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s">
         <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F43" t="s">
         <v>9</v>
@@ -2012,24 +2016,24 @@
         <v>1653.37</v>
       </c>
       <c r="I43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
         <v>160</v>
       </c>
       <c r="E44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
@@ -2041,7 +2045,7 @@
         <v>1581.64</v>
       </c>
       <c r="I44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2052,314 +2056,347 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBAF722-6FF6-47E8-8911-72262127743F}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1">
-        <f ca="1">RAND()*(2000-350)+350</f>
-        <v>877.87957536356907</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B43" ca="1" si="0">RAND()*(2000-350)+350</f>
-        <v>581.24034097780225</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <f t="shared" ca="1" si="0"/>
-        <v>1298.6371717057796</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>463.95303202113587</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1735.070616811782</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1208.0420997450346</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B7">
-        <f t="shared" ca="1" si="0"/>
-        <v>1410.7275701972039</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <f t="shared" ca="1" si="0"/>
-        <v>648.14718674247342</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B9">
-        <f t="shared" ca="1" si="0"/>
-        <v>578.00452573488678</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B10">
-        <f t="shared" ca="1" si="0"/>
-        <v>1245.6190099221055</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1435.6687308547127</v>
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B13">
-        <f t="shared" ca="1" si="0"/>
-        <v>1869.814297623928</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <f t="shared" ca="1" si="0"/>
-        <v>1675.298908191161</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B15">
-        <f t="shared" ca="1" si="0"/>
-        <v>1303.4462312852572</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B16">
-        <f t="shared" ca="1" si="0"/>
-        <v>363.96063657761772</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
       <c r="B17">
-        <f t="shared" ca="1" si="0"/>
-        <v>1490.0695134279913</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
       <c r="B18">
-        <f t="shared" ca="1" si="0"/>
-        <v>1768.0163517392532</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
       <c r="B19">
-        <f t="shared" ca="1" si="0"/>
-        <v>1590.1270518767369</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
       <c r="B20">
-        <f t="shared" ca="1" si="0"/>
-        <v>1220.8920743991953</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
       <c r="B21">
-        <f t="shared" ca="1" si="0"/>
-        <v>1349.1893892652342</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <f t="shared" ca="1" si="0"/>
-        <v>1597.6158381411733</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
       <c r="B24">
-        <f t="shared" ca="1" si="0"/>
-        <v>786.03558231101931</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
       <c r="B25">
-        <f t="shared" ca="1" si="0"/>
-        <v>1046.8582600728764</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
       <c r="B26">
-        <f t="shared" ca="1" si="0"/>
-        <v>959.06517249342835</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
       <c r="B27">
-        <f t="shared" ca="1" si="0"/>
-        <v>1277.4598680791332</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
       <c r="B28">
-        <f t="shared" ca="1" si="0"/>
-        <v>919.98545775370917</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
       <c r="B29">
-        <f t="shared" ca="1" si="0"/>
-        <v>896.12976870053058</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>83</v>
+      </c>
       <c r="B30">
-        <f t="shared" ca="1" si="0"/>
-        <v>571.0723892973017</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
       <c r="B31">
-        <f t="shared" ca="1" si="0"/>
-        <v>1956.5233871824266</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
       <c r="B32">
-        <f t="shared" ca="1" si="0"/>
-        <v>421.3541445933742</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <f t="shared" ca="1" si="0"/>
-        <v>802.39479104973088</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
       <c r="B35">
-        <f t="shared" ca="1" si="0"/>
-        <v>1446.4748182649814</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
       <c r="B36">
-        <f t="shared" ca="1" si="0"/>
-        <v>518.48992646314218</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
       <c r="B37">
-        <f t="shared" ca="1" si="0"/>
-        <v>1322.8366291957575</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>109</v>
+      </c>
       <c r="B38">
-        <f t="shared" ca="1" si="0"/>
-        <v>977.96062631390475</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
       <c r="B39">
-        <f t="shared" ca="1" si="0"/>
-        <v>1363.2000736165196</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
       <c r="B40">
-        <f t="shared" ca="1" si="0"/>
-        <v>717.39221279829314</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
       <c r="B41">
-        <f t="shared" ca="1" si="0"/>
-        <v>1966.5854545886291</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>110</v>
+      </c>
       <c r="B42">
-        <f t="shared" ca="1" si="0"/>
-        <v>1137.1256263448074</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>112</v>
+      </c>
       <c r="B43">
-        <f t="shared" ca="1" si="0"/>
-        <v>988.6636431659407</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A16" xr:uid="{4EC55469-5405-402B-9A57-EFAEAC9B74E8}">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>